<commit_message>
batch writting data back to Excel with only READ and WRITE file once.
</commit_message>
<xml_diff>
--- a/target/test-classes/TestCase_v7.xlsx
+++ b/target/test-classes/TestCase_v7.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaa./Documents/project/apiAuto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7099802F-203B-C640-9557-A1F628BC66D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="8_{7099802F-203B-C640-9557-A1F628BC66D1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="800" windowWidth="27440" windowHeight="16540" activeTab="1" xr2:uid="{C2C68A0E-8208-CB4E-A46B-1F8D63907E68}"/>
+    <workbookView activeTab="1" windowHeight="16540" windowWidth="27440" xWindow="1620" xr2:uid="{C2C68A0E-8208-CB4E-A46B-1F8D63907E68}" yWindow="800"/>
   </bookViews>
   <sheets>
-    <sheet name="ApiInfoSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Case2" sheetId="2" r:id="rId2"/>
+    <sheet name="ApiInfoSheet" r:id="rId1" sheetId="1"/>
+    <sheet name="Case2" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>CaseId(用例编号)</t>
   </si>
@@ -214,12 +214,16 @@
   </si>
   <si>
     <t>ActualResponseData(实际响应数值)</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -247,19 +251,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -276,10 +280,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -314,7 +318,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -366,7 +370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -477,21 +481,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -508,7 +512,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -560,15 +564,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3C0F18-4128-E243-8FFF-504C5D1B27A8}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3C0F18-4128-E243-8FFF-504C5D1B27A8}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
@@ -576,10 +580,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="69.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="69.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -779,13 +783,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DB5EC3-A329-1C44-BF0B-E5AF52B9ED1D}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DB5EC3-A329-1C44-BF0B-E5AF52B9ED1D}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -793,12 +797,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="72.5" customWidth="1"/>
-    <col min="6" max="6" width="53.83203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="46.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="72.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="53.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -837,6 +841,9 @@
       <c r="E2" t="s">
         <v>53</v>
       </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -854,6 +861,9 @@
       <c r="E3" t="s">
         <v>54</v>
       </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -871,6 +881,9 @@
       <c r="E4" t="s">
         <v>55</v>
       </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -888,6 +901,9 @@
       <c r="E5" t="s">
         <v>56</v>
       </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -905,6 +921,9 @@
       <c r="E6" t="s">
         <v>57</v>
       </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -922,6 +941,9 @@
       <c r="E7" t="s">
         <v>57</v>
       </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -939,6 +961,9 @@
       <c r="E8" t="s">
         <v>53</v>
       </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -956,6 +981,9 @@
       <c r="E9" t="s">
         <v>54</v>
       </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -973,6 +1001,9 @@
       <c r="E10" t="s">
         <v>58</v>
       </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -990,6 +1021,9 @@
       <c r="E11" t="s">
         <v>58</v>
       </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1007,8 +1041,11 @@
       <c r="E12" t="s">
         <v>59</v>
       </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>